<commit_message>
Updated simulation and summary
Simulation now uses actual 3D leg model while running
Executive summary for dynamic simulation updated
</commit_message>
<xml_diff>
--- a/System Modelling/Mechanical/Agile Controls Simulation/ParameterConfig.xlsx
+++ b/System Modelling/Mechanical/Agile Controls Simulation/ParameterConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Documents\GitHub\AgileRoboticControls\Software\Agile Controls Simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Documents\GitHub\AgileRoboticControls\System Modelling\Mechanical\Agile Controls Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -640,7 +640,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>